<commit_message>
scripts creating nationalist vote share and death maps
</commit_message>
<xml_diff>
--- a/Data/municipality_reorg.xlsx
+++ b/Data/municipality_reorg.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmyballesteros/R/bih_voting/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1811D41E-8EE6-4C4E-BE35-194836B66378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F588E0F-A305-D545-BD19-674F93AA1CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11040" yWindow="760" windowWidth="23520" windowHeight="20880" xr2:uid="{1583C5B0-675C-EB4F-AB25-FB832508D634}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="161">
   <si>
     <t>Pre-War Municipality</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Krupa na Uni</t>
   </si>
   <si>
-    <t>Novi Grad</t>
-  </si>
-  <si>
-    <t>Kostajnica</t>
-  </si>
-  <si>
     <t>Sanski Most</t>
   </si>
   <si>
@@ -80,12 +74,6 @@
     <t>Drvar</t>
   </si>
   <si>
-    <t>Kupres (RS)</t>
-  </si>
-  <si>
-    <t>Kupres (BiH)</t>
-  </si>
-  <si>
     <t>Kupres</t>
   </si>
   <si>
@@ -95,18 +83,9 @@
     <t>Jajce</t>
   </si>
   <si>
-    <t>Kneževo</t>
-  </si>
-  <si>
-    <t>Dobrotići</t>
-  </si>
-  <si>
     <t>Mostar</t>
   </si>
   <si>
-    <t>Istočni Nostar</t>
-  </si>
-  <si>
     <t>Berkovići</t>
   </si>
   <si>
@@ -128,9 +107,6 @@
     <t>Goražde</t>
   </si>
   <si>
-    <t>Novi Goražde</t>
-  </si>
-  <si>
     <t>Pale</t>
   </si>
   <si>
@@ -143,9 +119,6 @@
     <t>Istočna Ilidža</t>
   </si>
   <si>
-    <t>Stari Grad</t>
-  </si>
-  <si>
     <t>Istočni Stari Grad</t>
   </si>
   <si>
@@ -206,24 +179,12 @@
     <t>Doboj</t>
   </si>
   <si>
-    <t>Doboj Istok</t>
-  </si>
-  <si>
-    <t>Doboj Jug</t>
-  </si>
-  <si>
     <t>Usora</t>
   </si>
   <si>
     <t>Tešanj</t>
   </si>
   <si>
-    <t>Trnovo (BiH)</t>
-  </si>
-  <si>
-    <t>Trnovo (RS)</t>
-  </si>
-  <si>
     <t>Trnovo</t>
   </si>
   <si>
@@ -473,30 +434,15 @@
     <t>Živinice</t>
   </si>
   <si>
-    <t>Kozarska Dubica</t>
-  </si>
-  <si>
-    <t>Gradiška</t>
-  </si>
-  <si>
-    <t>Brod</t>
-  </si>
-  <si>
     <t>Bijeljina</t>
   </si>
   <si>
-    <t>Živinive</t>
-  </si>
-  <si>
     <t>Prozor-Rama</t>
   </si>
   <si>
     <t>Gornji Vakuf-Uskoplje</t>
   </si>
   <si>
-    <t>Istočno Novo Sarajevo</t>
-  </si>
-  <si>
     <t>Novo Sarajevo</t>
   </si>
   <si>
@@ -513,13 +459,73 @@
   </si>
   <si>
     <t>Modified</t>
+  </si>
+  <si>
+    <t>Kupres-FBIH</t>
+  </si>
+  <si>
+    <t>Dobretići</t>
+  </si>
+  <si>
+    <t>Centar Sarajevo</t>
+  </si>
+  <si>
+    <t>Novi Grad Sarajevo</t>
+  </si>
+  <si>
+    <t>Stari Grad Sarajevo</t>
+  </si>
+  <si>
+    <t>Trnovo-FBIH</t>
+  </si>
+  <si>
+    <t>Vogošća</t>
+  </si>
+  <si>
+    <t>Doboj East</t>
+  </si>
+  <si>
+    <t>Doboj South</t>
+  </si>
+  <si>
+    <t>Bosanska Gradiška</t>
+  </si>
+  <si>
+    <t>Bosanska Kostajnica</t>
+  </si>
+  <si>
+    <t>Dubica</t>
+  </si>
+  <si>
+    <t>Kupres-RS</t>
+  </si>
+  <si>
+    <t>Novi Grad</t>
+  </si>
+  <si>
+    <t>Skender Vakuf / Kneževo</t>
+  </si>
+  <si>
+    <t>Bosanski Brod</t>
+  </si>
+  <si>
+    <t>Novo Goražde</t>
+  </si>
+  <si>
+    <t>East New Sarajevo</t>
+  </si>
+  <si>
+    <t>Trnovo-RS</t>
+  </si>
+  <si>
+    <t>Istočni Mostar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -532,6 +538,25 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -554,19 +579,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,547 +928,572 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA4A2A1-F0F1-4640-88FE-98F8D7E3F45D}">
-  <dimension ref="A1:F176"/>
+  <dimension ref="A1:G176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="42.5" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>60</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="B32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="B33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="B34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="B38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="G39" s="7"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="7"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="C46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C35" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C36" s="1">
-        <v>1</v>
-      </c>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="C48" s="1">
         <v>1</v>
@@ -1449,10 +1501,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="C49" s="1">
         <v>1</v>
@@ -1460,54 +1512,54 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C50" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>51</v>
+        <v>27</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="C51" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>51</v>
+    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>53</v>
+        <v>81</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="C53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="C54" s="1">
         <v>1</v>
@@ -1515,192 +1567,192 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="C55" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>55</v>
+        <v>82</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="C56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C57" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>59</v>
+        <v>83</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="C58" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>59</v>
+        <v>84</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="C59" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>62</v>
+        <v>85</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="C60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="C61" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C62" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C63" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C64" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C65" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="B66" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C66" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
-        <v>64</v>
+      <c r="A67" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="C67" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
-        <v>65</v>
+      <c r="A68" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="C68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
     </row>
-    <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>66</v>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C69" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
     </row>
-    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>67</v>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C70" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
     </row>
     <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
-        <v>73</v>
+      <c r="A71" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="C71" s="1">
         <v>0</v>
@@ -1709,11 +1761,11 @@
       <c r="E71" s="3"/>
     </row>
     <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
-        <v>74</v>
+      <c r="A72" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="C72" s="1">
         <v>0</v>
@@ -1722,11 +1774,11 @@
       <c r="E72" s="3"/>
     </row>
     <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
-        <v>75</v>
+      <c r="A73" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C73" s="1">
         <v>0</v>
@@ -1735,11 +1787,11 @@
       <c r="E73" s="3"/>
     </row>
     <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
-        <v>76</v>
+      <c r="A74" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C74" s="1">
         <v>0</v>
@@ -1747,25 +1799,25 @@
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
     </row>
-    <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>70</v>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C75" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
     </row>
     <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
-        <v>77</v>
+      <c r="A76" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C76" s="1">
         <v>0</v>
@@ -1774,11 +1826,11 @@
       <c r="E76" s="3"/>
     </row>
     <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>78</v>
+      <c r="A77" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="C77" s="1">
         <v>0</v>
@@ -1786,25 +1838,25 @@
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
     </row>
-    <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>79</v>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C78" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
     </row>
     <row r="79" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
-        <v>80</v>
+      <c r="A79" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="C79" s="1">
         <v>0</v>
@@ -1812,25 +1864,25 @@
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
     </row>
-    <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>81</v>
+        <v>15</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C80" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
     </row>
     <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
-        <v>82</v>
+      <c r="A81" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C81" s="1">
         <v>0</v>
@@ -1839,11 +1891,11 @@
       <c r="E81" s="3"/>
     </row>
     <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
-        <v>83</v>
+      <c r="A82" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="C82" s="1">
         <v>0</v>
@@ -1852,11 +1904,11 @@
       <c r="E82" s="3"/>
     </row>
     <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
-        <v>84</v>
+      <c r="A83" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="C83" s="1">
         <v>0</v>
@@ -1864,38 +1916,38 @@
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
     </row>
-    <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>85</v>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C84" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
     </row>
     <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
-        <v>86</v>
+      <c r="A85" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="C85" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
     </row>
     <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
-        <v>87</v>
+      <c r="A86" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C86" s="1">
         <v>0</v>
@@ -1904,37 +1956,37 @@
       <c r="E86" s="3"/>
     </row>
     <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
-        <v>88</v>
+      <c r="A87" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
       <c r="C87" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
     </row>
-    <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>89</v>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="C88" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
     </row>
     <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="s">
-        <v>146</v>
+      <c r="A89" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="C89" s="1">
         <v>0</v>
@@ -1942,116 +1994,116 @@
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
     </row>
-    <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>90</v>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C90" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
     </row>
-    <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>91</v>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C91" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
     </row>
-    <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>92</v>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C92" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
     </row>
-    <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>93</v>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C93" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
     </row>
-    <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>94</v>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C94" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
     </row>
-    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>95</v>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="C95" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
     </row>
     <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="4" t="s">
-        <v>96</v>
+      <c r="A96" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="C96" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
     </row>
-    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>97</v>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C97" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
     </row>
     <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" s="4" t="s">
-        <v>98</v>
+      <c r="A98" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C98" s="1">
         <v>0</v>
@@ -2060,11 +2112,11 @@
       <c r="E98" s="3"/>
     </row>
     <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="4" t="s">
-        <v>99</v>
+      <c r="A99" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C99" s="1">
         <v>0</v>
@@ -2073,11 +2125,11 @@
       <c r="E99" s="3"/>
     </row>
     <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="4" t="s">
-        <v>100</v>
+      <c r="A100" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C100" s="1">
         <v>0</v>
@@ -2086,11 +2138,11 @@
       <c r="E100" s="3"/>
     </row>
     <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A101" s="4" t="s">
-        <v>145</v>
+      <c r="A101" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="C101" s="1">
         <v>0</v>
@@ -2098,38 +2150,38 @@
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
     </row>
-    <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>101</v>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C102" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
     </row>
-    <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>102</v>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C103" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
     </row>
     <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="4" t="s">
-        <v>103</v>
+      <c r="A104" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C104" s="1">
         <v>0</v>
@@ -2138,11 +2190,11 @@
       <c r="E104" s="3"/>
     </row>
     <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" s="4" t="s">
-        <v>104</v>
+      <c r="A105" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C105" s="1">
         <v>0</v>
@@ -2151,50 +2203,50 @@
       <c r="E105" s="3"/>
     </row>
     <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="4" t="s">
-        <v>105</v>
+      <c r="A106" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="C106" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
     </row>
-    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>106</v>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C107" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
     </row>
-    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>108</v>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C108" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
     </row>
     <row r="109" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="4" t="s">
-        <v>109</v>
+      <c r="A109" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C109" s="1">
         <v>0</v>
@@ -2203,11 +2255,11 @@
       <c r="E109" s="3"/>
     </row>
     <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
-        <v>110</v>
+      <c r="A110" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C110" s="1">
         <v>0</v>
@@ -2216,11 +2268,11 @@
       <c r="E110" s="3"/>
     </row>
     <row r="111" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A111" s="4" t="s">
-        <v>111</v>
+      <c r="A111" s="5" t="s">
+        <v>147</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C111" s="1">
         <v>0</v>
@@ -2229,11 +2281,11 @@
       <c r="E111" s="3"/>
     </row>
     <row r="112" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A112" s="4" t="s">
-        <v>121</v>
+      <c r="A112" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C112" s="1">
         <v>0</v>
@@ -2242,7 +2294,7 @@
       <c r="E112" s="3"/>
     </row>
     <row r="113" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A113" s="4" t="s">
+      <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
@@ -2255,7 +2307,7 @@
       <c r="E113" s="3"/>
     </row>
     <row r="114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A114" s="4" t="s">
+      <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
@@ -2268,11 +2320,11 @@
       <c r="E114" s="3"/>
     </row>
     <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A115" s="4" t="s">
-        <v>114</v>
+      <c r="A115" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C115" s="1">
         <v>0</v>
@@ -2281,11 +2333,11 @@
       <c r="E115" s="3"/>
     </row>
     <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A116" s="4" t="s">
-        <v>115</v>
+      <c r="A116" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C116" s="1">
         <v>0</v>
@@ -2294,11 +2346,11 @@
       <c r="E116" s="3"/>
     </row>
     <row r="117" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A117" s="4" t="s">
-        <v>116</v>
+      <c r="A117" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C117" s="1">
         <v>0</v>
@@ -2307,11 +2359,11 @@
       <c r="E117" s="3"/>
     </row>
     <row r="118" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A118" s="4" t="s">
-        <v>150</v>
+      <c r="A118" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C118" s="1">
         <v>0</v>
@@ -2320,63 +2372,63 @@
       <c r="E118" s="3"/>
     </row>
     <row r="119" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A119" s="4" t="s">
-        <v>118</v>
+      <c r="A119" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C119" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
     </row>
-    <row r="120" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>119</v>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C120" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
     </row>
-    <row r="121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>124</v>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C121" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
     </row>
-    <row r="122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>125</v>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C122" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
     </row>
     <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A123" s="4" t="s">
-        <v>126</v>
+      <c r="A123" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C123" s="1">
         <v>0</v>
@@ -2385,11 +2437,11 @@
       <c r="E123" s="3"/>
     </row>
     <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A124" s="4" t="s">
-        <v>128</v>
+      <c r="A124" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C124" s="1">
         <v>0</v>
@@ -2398,11 +2450,11 @@
       <c r="E124" s="3"/>
     </row>
     <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A125" s="4" t="s">
-        <v>129</v>
+      <c r="A125" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C125" s="1">
         <v>0</v>
@@ -2410,51 +2462,51 @@
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
     </row>
-    <row r="126" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A126" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>130</v>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C126" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
     </row>
-    <row r="127" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A127" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>131</v>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
     </row>
-    <row r="128" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A128" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>132</v>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C128" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
     </row>
     <row r="129" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A129" s="4" t="s">
-        <v>133</v>
+      <c r="A129" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C129" s="1">
         <v>0</v>
@@ -2462,38 +2514,38 @@
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
     </row>
-    <row r="130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A130" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>134</v>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C130" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
     </row>
-    <row r="131" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A131" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>135</v>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C131" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D131" s="3"/>
       <c r="E131" s="3"/>
     </row>
     <row r="132" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A132" s="4" t="s">
-        <v>136</v>
+      <c r="A132" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="C132" s="1">
         <v>0</v>
@@ -2503,10 +2555,10 @@
     </row>
     <row r="133" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="C133" s="1">
         <v>0</v>
@@ -2515,11 +2567,11 @@
       <c r="E133" s="3"/>
     </row>
     <row r="134" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A134" s="4" t="s">
-        <v>138</v>
+      <c r="A134" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="C134" s="1">
         <v>0</v>
@@ -2528,11 +2580,11 @@
       <c r="E134" s="3"/>
     </row>
     <row r="135" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A135" s="4" t="s">
-        <v>139</v>
+      <c r="A135" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C135" s="1">
         <v>0</v>
@@ -2541,11 +2593,11 @@
       <c r="E135" s="3"/>
     </row>
     <row r="136" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A136" s="4" t="s">
-        <v>140</v>
+      <c r="A136" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="C136" s="1">
         <v>0</v>
@@ -2553,38 +2605,38 @@
       <c r="D136" s="3"/>
       <c r="E136" s="3"/>
     </row>
-    <row r="137" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A137" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>123</v>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C137" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D137" s="3"/>
       <c r="E137" s="3"/>
     </row>
-    <row r="138" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A138" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>141</v>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="C138" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D138" s="3"/>
       <c r="E138" s="3"/>
     </row>
     <row r="139" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A139" s="4" t="s">
-        <v>142</v>
+      <c r="A139" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="C139" s="1">
         <v>0</v>
@@ -2593,11 +2645,11 @@
       <c r="E139" s="3"/>
     </row>
     <row r="140" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A140" s="4" t="s">
-        <v>143</v>
+      <c r="A140" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C140" s="1">
         <v>0</v>
@@ -2606,11 +2658,11 @@
       <c r="E140" s="3"/>
     </row>
     <row r="141" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A141" s="4" t="s">
-        <v>149</v>
+      <c r="A141" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="C141" s="1">
         <v>0</v>
@@ -2619,11 +2671,11 @@
       <c r="E141" s="3"/>
     </row>
     <row r="142" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A142" s="4" t="s">
-        <v>120</v>
+      <c r="A142" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="C142" s="1">
         <v>0</v>
@@ -2631,15 +2683,15 @@
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
     </row>
-    <row r="143" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A143" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B143" s="5" t="s">
-        <v>107</v>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C143" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D143" s="3"/>
       <c r="E143" s="3"/>
@@ -2843,8 +2895,8 @@
       <c r="E176" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F27:F90">
-    <sortCondition ref="F90"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C143">
+    <sortCondition ref="A2:A143"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>